<commit_message>
Updated the test case excel sheet.
</commit_message>
<xml_diff>
--- a/vendor/grt_application_testcase.xlsx
+++ b/vendor/grt_application_testcase.xlsx
@@ -34,28 +34,9 @@
     <t>Fetch the details for user having twitter account only</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Go to </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <color rgb="000000FF"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">http://morning-fortress-1241.herokuapp.com
-</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">2. Enter a user name for e.g beingsalmankhan
+    <t>1. Go to http://morning-fortress-1241.herokuapp.com
+2. Enter a user name for e.g beingsalmankhan
 3. Click on search</t>
-    </r>
   </si>
   <si>
     <t>1. Search will fetch 10 tweets from twitter account
@@ -66,28 +47,9 @@
     <t>Fetch the details for user having github account only</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Go to </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <color rgb="000000FF"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">http://morning-fortress-1241.herokuapp.com
-</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">2. Enter a user name [Having acount only in Github.com]
+    <t>1. Go to http://morning-fortress-1241.herokuapp.com
+2. Enter a user name [Having acount only in Github.com]
 3. Click on search</t>
-    </r>
   </si>
   <si>
     <t>1. Search will fetch following details from github account
@@ -101,28 +63,9 @@
     <t>Fetch the details for user having rubygems account only</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Go to </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <color rgb="000000FF"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">http://morning-fortress-1241.herokuapp.com</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve"> 
+    <t>1. Go to http://morning-fortress-1241.herokuapp.com 
 2. Enter a user name [Having account in rubygems.org]
 3. Click on search</t>
-    </r>
   </si>
   <si>
     <t>1. Search will fetch number on gems build by the users
@@ -133,28 +76,9 @@
     <t>Fetch details from twitter &amp; github account</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Go to </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <color rgb="000000FF"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">http://morning-fortress-1241.herokuapp.com</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">  
+    <t>1. Go to http://morning-fortress-1241.herokuapp.com  
 2. Enter a user name [Having account in both the websites]
 3. Click on search</t>
-    </r>
   </si>
   <si>
     <t>1. Search will fetch 10 tweets from twitter account 
@@ -168,28 +92,9 @@
     <t>Fetch details from twitter &amp; Rubygems account</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Go to </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <color rgb="000000FF"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">http://morning-fortress-1241.herokuapp.com</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve"> 
+    <t>1. Go to http://morning-fortress-1241.herokuapp.com 
 2. Enter a user name [Having acount in both the websites] 
 3. Click on search</t>
-    </r>
   </si>
   <si>
     <t>1. Search will fetch 10 tweets from twitter account 
@@ -211,28 +116,9 @@
     <t>Fetch details from all the 3 websites</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Go to </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <color rgb="000000FF"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">http://morning-fortress-1241.herokuapp.com
-</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">2. Enter a user name for e.g. Sferik
+    <t>1. Go to http://morning-fortress-1241.herokuapp.com
+2. Enter a user name for e.g. Sferik
  3. Click on search</t>
-    </r>
   </si>
   <si>
     <t>1. Search will fetch 10 tweets from twitter account 
@@ -246,30 +132,11 @@
     <t>Export details to PDF</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Go to </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <color rgb="000000FF"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">http://morning-fortress-1241.herokuapp.com</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve"> 
+    <t>1. Go to http://morning-fortress-1241.herokuapp.com 
 2. Enter a user name 
 3. Click on search
 4. On the results page, click on 'Export to' select box
 5. select 'PDF' option</t>
-    </r>
   </si>
   <si>
     <t>It will generate a PDF file with name '&lt;username&gt;.pdf' having all 
@@ -279,105 +146,29 @@
     <t>Export details to DOC</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Go to </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <color rgb="000000FF"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">http://morning-fortress-1241.herokuapp.com</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve"> 
+    <t>1. Go to http://morning-fortress-1241.herokuapp.com 
 2. Enter a user name  
 3. Click on search
 4. On the results page, click on 'Export to' select box
 5. select 'DOC' option</t>
-    </r>
   </si>
   <si>
     <t>It will generate a DOC file with name '&lt;username&gt;.doc' having all
  The data displayed on the results page</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Return to home page [</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <color rgb="000000FF"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">http://morning-fortress-1241.herokuapp.com</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">] 
+    <t>Return to home page [http://morning-fortress-1241.herokuapp.com] 
 on clicking 'Back' button on results page</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Go to </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <color rgb="000000FF"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">http://morning-fortress-1241.herokuapp.com</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve"> 
+  </si>
+  <si>
+    <t>1. Go to http://morning-fortress-1241.herokuapp.com 
 2. Enter a user name 
 3. Click on search
 4. On the results page, click on 'Back' button</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Browser will return to the home page
- [</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <color rgb="000000FF"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">http://morning-fortress-1241.herokuapp.com</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">]</t>
-    </r>
+  </si>
+  <si>
+    <t>Browser will return to the home page
+ [http://morning-fortress-1241.herokuapp.com]</t>
   </si>
 </sst>
 </file>
@@ -387,9 +178,10 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -410,14 +202,9 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <color rgb="000000FF"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -576,18 +363,18 @@
   <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="C5"/>
+      <selection activeCell="D13" activeCellId="0" pane="topLeft" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.0392156862745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.6078431372549"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.0862745098039"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.7764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.356862745098"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2" s="4">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2" s="4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -601,7 +388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="35.05" outlineLevel="0" r="3">
       <c r="A3" s="5" t="n">
         <v>1</v>
       </c>
@@ -615,7 +402,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="68.65" outlineLevel="0" r="4">
       <c r="A4" s="5" t="n">
         <v>2</v>
       </c>
@@ -629,7 +416,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="35.05" outlineLevel="0" r="5">
       <c r="A5" s="5" t="n">
         <v>3</v>
       </c>
@@ -643,7 +430,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="68.65" outlineLevel="0" r="6">
       <c r="A6" s="5" t="n">
         <v>4</v>
       </c>
@@ -657,7 +444,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="35.05" outlineLevel="0" r="7">
       <c r="A7" s="5" t="n">
         <v>5</v>
       </c>
@@ -671,7 +458,7 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="68.65" outlineLevel="0" r="8">
       <c r="A8" s="5" t="n">
         <v>6</v>
       </c>
@@ -685,7 +472,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="68.65" outlineLevel="0" r="9">
       <c r="A9" s="5" t="n">
         <v>7</v>
       </c>
@@ -699,7 +486,7 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="57.45" outlineLevel="0" r="10">
       <c r="A10" s="5" t="n">
         <v>8</v>
       </c>
@@ -713,7 +500,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="57.45" outlineLevel="0" r="11">
       <c r="A11" s="5" t="n">
         <v>9</v>
       </c>
@@ -727,7 +514,7 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="46.25" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="46.25" outlineLevel="0" r="12">
       <c r="A12" s="5" t="n">
         <v>10</v>
       </c>
@@ -742,20 +529,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink display="http://morning-fortress-1241.herokuapp.com" ref="C3" r:id="rId1"/>
-    <hyperlink display="http://morning-fortress-1241.herokuapp.com" ref="C4" r:id="rId2"/>
-    <hyperlink display="http://morning-fortress-1241.herokuapp.com" ref="C5" r:id="rId3"/>
-    <hyperlink display="http://morning-fortress-1241.herokuapp.com" ref="C6" r:id="rId4"/>
-    <hyperlink display="http://morning-fortress-1241.herokuapp.com" ref="C7" r:id="rId5"/>
-    <hyperlink display="http://morning-fortress-1241.herokuapp.com" ref="C8" r:id="rId6"/>
-    <hyperlink display="http://morning-fortress-1241.herokuapp.com" ref="C9" r:id="rId7"/>
-    <hyperlink display="http://morning-fortress-1241.herokuapp.com" ref="C10" r:id="rId8"/>
-    <hyperlink display="http://morning-fortress-1241.herokuapp.com" ref="C11" r:id="rId9"/>
-    <hyperlink display="http://morning-fortress-1241.herokuapp.com" ref="B12" r:id="rId10"/>
-    <hyperlink display="http://morning-fortress-1241.herokuapp.com" ref="C12" r:id="rId11"/>
-    <hyperlink display="http://morning-fortress-1241.herokuapp.com" ref="D12" r:id="rId12"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
@@ -773,17 +546,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -798,17 +571,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>